<commit_message>
FOL example part 1
</commit_message>
<xml_diff>
--- a/AI and ML.xlsx
+++ b/AI and ML.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="209">
   <si>
     <t>Machine Learning</t>
   </si>
@@ -333,6 +333,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Rule: </t>
     </r>
     <r>
@@ -459,6 +467,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t>Objects</t>
     </r>
     <r>
@@ -526,16 +542,326 @@
   <si>
     <t>7. Debug the knowledge base and eliminate errors</t>
   </si>
+  <si>
+    <t>Step 1:</t>
+  </si>
+  <si>
+    <t>Identify the task / problem:</t>
+  </si>
+  <si>
+    <t>1. Identify the function/output of the circuit based on the inputs</t>
+  </si>
+  <si>
+    <t>2. Check if there are any feedback loops.</t>
+  </si>
+  <si>
+    <t>3. Investigate delays and power consumptions (Optional)</t>
+  </si>
+  <si>
+    <t>Step 2:</t>
+  </si>
+  <si>
+    <t>Collect relevant Know How:</t>
+  </si>
+  <si>
+    <t>1. Digital circuits are made of logic gates and wires</t>
+  </si>
+  <si>
+    <t>2. Signals are sent via wire to the inputs of the Gates.</t>
+  </si>
+  <si>
+    <t>3. Gates processes the signals to produce output.</t>
+  </si>
+  <si>
+    <t>4. Four types of Gates to consider OR, AND, XOR and NOT.</t>
+  </si>
+  <si>
+    <t>5. OR, AND and XOR gates have two inputs and one output each. NOT has one input and one output.</t>
+  </si>
+  <si>
+    <t>6. We can neglect the effect of wires and focus on only inputs and outputs of gates for the simplicity.</t>
+  </si>
+  <si>
+    <t>Step 3:</t>
+  </si>
+  <si>
+    <t>Define the vocabulary:</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Constants</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: In order to make Gates distinguishable, we map the gates to constants e.g. X1, X2, ...</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Functions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The functioning of the Gate is dependent on its type, so we define a function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> which tells us exactly that. e.g. Type(X1) = XOR.</t>
+    </r>
+  </si>
+  <si>
+    <t>We define functions IN and OUT for input and output. e.g IN(1, X1) means 1st input of X1, OUT(1, A1) means 1st output of A1.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Signal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> can be used to denote that a certain variable represents a signal. e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Signal(t)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> means t is a signal.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Predicate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The connection between two gates is a relation between two gates, so it can be defined using a predicate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Connected.</t>
+    </r>
+  </si>
+  <si>
+    <t>E.g.: Connected(Out(1, X1), IN(2, A2)) tells that Output 1 of X1 is connected to Input 2 of A2.</t>
+  </si>
+  <si>
+    <t>5. Constants 0 and 1 should be used to indicate signals 0 and 1.</t>
+  </si>
+  <si>
+    <t>Step 4:</t>
+  </si>
+  <si>
+    <t>Encode General Knowledge of Domain:</t>
+  </si>
+  <si>
+    <t>1. If two inputs or outputs are connected, they share the signal:</t>
+  </si>
+  <si>
+    <t>A t1, t2 Connected(t1, t2) =&gt; Signal(t1) = Signal(t2)</t>
+  </si>
+  <si>
+    <t>2. The signal can be either 0 or 1.</t>
+  </si>
+  <si>
+    <t>At Signal(t) = 0 ^ Signal(t) = 1</t>
+  </si>
+  <si>
+    <t>Adder Circuit
+ example</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3. The predicate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Connected</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is commutative:</t>
+    </r>
+  </si>
+  <si>
+    <t>A t1, t2 Connected(t1, t2) &lt;=&gt; Connected(t2, t1)</t>
+  </si>
+  <si>
+    <t>4. The output of an OR gate is 1, if and only if at least 1 input is 1.</t>
+  </si>
+  <si>
+    <t>A  g Type(g) = OR =&gt; Signal(Out(1, g) = 1 &lt;=&gt; En Signal(In(n, g)) = 1</t>
+  </si>
+  <si>
+    <t>5. The output of an AND gate is 0, if and only if at least one of the input is 0</t>
+  </si>
+  <si>
+    <t>A g Type(g) = AND =&gt; Signal(Out(1, g) = 0 &lt;=&gt; En Signal(In(n, g)) = 0</t>
+  </si>
+  <si>
+    <t>6. The output of an XOR gate is 1 if and only if both inputs differ</t>
+  </si>
+  <si>
+    <t>A g Type(g) = XOR =&gt; Signal(Out(1, g) = 1 &lt;=&gt; Signal(In(1, g)) != Signal(In(2, g))</t>
+  </si>
+  <si>
+    <t>7. The output of the NOT gate differs from its input</t>
+  </si>
+  <si>
+    <t>A g Type(g) = NOT =&gt; Signal(In(1, g)) != Signal(Out(1, g))</t>
+  </si>
+  <si>
+    <t>Step 5:</t>
+  </si>
+  <si>
+    <t>Encoding information specific to our problem</t>
+  </si>
+  <si>
+    <t>At this step, we encode information specific to our Adder Circuit</t>
+  </si>
+  <si>
+    <t>Type(X1) = XOR, Type(X2) = XOR, Type(A1) = AND, Type(A2) = AND, Type(O1) = OR</t>
+  </si>
+  <si>
+    <t>Connected(In(1, X1), In(1, C))</t>
+  </si>
+  <si>
+    <t>C is input 1 of overall circuit</t>
+  </si>
+  <si>
+    <t>Connected(Out(1, X1), In(1, X2))</t>
+  </si>
+  <si>
+    <t>And so on...</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -556,52 +882,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -622,46 +903,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -676,7 +919,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -684,7 +927,67 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -697,6 +1000,29 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -707,187 +1033,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -898,6 +1224,51 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -921,6 +1292,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -936,45 +1316,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -983,180 +1324,174 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1">
       <alignment vertical="center"/>
@@ -1254,6 +1589,48 @@
         <a:xfrm>
           <a:off x="1341120" y="22296120"/>
           <a:ext cx="6751955" cy="3200400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>175</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>200</xdr:row>
+      <xdr:rowOff>122555</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="670560" y="29337000"/>
+          <a:ext cx="1744980" cy="4313555"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1587,7 +1964,7 @@
       </c>
     </row>
     <row r="14" spans="4:4">
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1623,12 +2000,12 @@
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="1"/>
       <c r="D24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
       <c r="G24" s="1" t="s">
         <v>19</v>
       </c>
@@ -1697,10 +2074,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A2:S173"/>
+  <dimension ref="A2:S221"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="Q150" sqref="Q150"/>
+    <sheetView tabSelected="1" topLeftCell="A192" workbookViewId="0">
+      <selection activeCell="F223" sqref="F223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2"/>
@@ -1732,7 +2109,7 @@
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="6" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1740,7 +2117,7 @@
       <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1748,17 +2125,17 @@
       <c r="C11" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="6" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="12" spans="5:5">
-      <c r="E12" s="3" t="s">
+      <c r="E12" s="6" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="13" spans="5:5">
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="6" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1766,7 +2143,7 @@
       <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="E16" s="6" t="s">
         <v>44</v>
       </c>
       <c r="I16" t="s">
@@ -1782,7 +2159,7 @@
       <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="6" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1833,16 +2210,16 @@
       </c>
     </row>
     <row r="31" spans="3:3">
-      <c r="C31" s="2"/>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="3:3">
-      <c r="C32" s="2"/>
+      <c r="C32" s="1"/>
     </row>
     <row r="33" spans="3:5">
       <c r="C33" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="6" t="s">
         <v>62</v>
       </c>
       <c r="E33" t="s">
@@ -1850,13 +2227,13 @@
       </c>
     </row>
     <row r="34" spans="3:3">
-      <c r="C34" s="2"/>
+      <c r="C34" s="1"/>
     </row>
     <row r="35" spans="3:8">
       <c r="C35" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="6" t="s">
         <v>62</v>
       </c>
       <c r="E35" t="s">
@@ -1867,13 +2244,13 @@
       </c>
     </row>
     <row r="36" spans="3:3">
-      <c r="C36" s="2"/>
+      <c r="C36" s="1"/>
     </row>
     <row r="37" spans="3:5">
       <c r="C37" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="6" t="s">
         <v>62</v>
       </c>
       <c r="E37" t="s">
@@ -1881,28 +2258,28 @@
       </c>
     </row>
     <row r="38" spans="3:3">
-      <c r="C38" s="2"/>
+      <c r="C38" s="1"/>
     </row>
     <row r="39" spans="3:5">
-      <c r="C39" s="2"/>
+      <c r="C39" s="1"/>
       <c r="E39" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="40" spans="3:5">
-      <c r="C40" s="2"/>
+      <c r="C40" s="1"/>
       <c r="E40" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="41" spans="3:3">
-      <c r="C41" s="2"/>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="3:5">
       <c r="C42" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="6" t="s">
         <v>62</v>
       </c>
       <c r="E42" t="s">
@@ -1910,25 +2287,25 @@
       </c>
     </row>
     <row r="43" spans="3:3">
-      <c r="C43" s="2"/>
+      <c r="C43" s="1"/>
     </row>
     <row r="44" spans="3:5">
-      <c r="C44" s="2"/>
+      <c r="C44" s="1"/>
       <c r="E44" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="45" spans="3:5">
-      <c r="C45" s="2"/>
+      <c r="C45" s="1"/>
       <c r="E45" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="46" spans="3:3">
-      <c r="C46" s="2"/>
+      <c r="C46" s="1"/>
     </row>
     <row r="47" spans="3:3">
-      <c r="C47" s="2"/>
+      <c r="C47" s="1"/>
     </row>
     <row r="48" spans="3:10">
       <c r="C48" s="1" t="s">
@@ -1942,7 +2319,7 @@
       </c>
     </row>
     <row r="49" spans="3:3">
-      <c r="C49" s="2"/>
+      <c r="C49" s="1"/>
     </row>
     <row r="50" spans="3:10">
       <c r="C50" s="1" t="s">
@@ -1956,10 +2333,10 @@
       </c>
     </row>
     <row r="51" spans="3:3">
-      <c r="C51" s="2"/>
+      <c r="C51" s="1"/>
     </row>
     <row r="52" spans="3:10">
-      <c r="C52" s="2"/>
+      <c r="C52" s="1"/>
       <c r="E52" t="s">
         <v>81</v>
       </c>
@@ -1968,10 +2345,10 @@
       </c>
     </row>
     <row r="53" spans="3:3">
-      <c r="C53" s="2"/>
+      <c r="C53" s="1"/>
     </row>
     <row r="54" spans="3:10">
-      <c r="C54" s="2"/>
+      <c r="C54" s="1"/>
       <c r="E54" t="s">
         <v>83</v>
       </c>
@@ -1980,16 +2357,16 @@
       </c>
     </row>
     <row r="55" spans="3:10">
-      <c r="C55" s="2"/>
+      <c r="C55" s="1"/>
       <c r="J55" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="56" spans="3:3">
-      <c r="C56" s="2"/>
+      <c r="C56" s="1"/>
     </row>
     <row r="57" spans="3:3">
-      <c r="C57" s="2"/>
+      <c r="C57" s="1"/>
     </row>
     <row r="58" spans="3:5">
       <c r="C58" s="1" t="s">
@@ -2000,13 +2377,13 @@
       </c>
     </row>
     <row r="59" spans="3:5">
-      <c r="C59" s="2"/>
+      <c r="C59" s="1"/>
       <c r="E59" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="60" spans="3:10">
-      <c r="C60" s="2"/>
+      <c r="C60" s="1"/>
       <c r="E60" t="s">
         <v>89</v>
       </c>
@@ -2015,13 +2392,13 @@
       </c>
     </row>
     <row r="61" spans="3:3">
-      <c r="C61" s="2"/>
+      <c r="C61" s="1"/>
     </row>
     <row r="66" spans="3:5">
       <c r="C66" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E66" s="3" t="s">
+      <c r="E66" s="6" t="s">
         <v>91</v>
       </c>
     </row>
@@ -2029,13 +2406,13 @@
       <c r="C67" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E67" s="3" t="s">
+      <c r="E67" s="6" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="68" spans="3:5">
-      <c r="C68" s="2"/>
-      <c r="E68" s="3" t="s">
+      <c r="C68" s="1"/>
+      <c r="E68" s="6" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2043,48 +2420,48 @@
       <c r="C69" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E69" s="3" t="s">
+      <c r="E69" s="6" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="70" spans="3:3">
-      <c r="C70" s="2"/>
+      <c r="C70" s="1"/>
     </row>
     <row r="71" spans="3:5">
       <c r="C71" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E71" s="3" t="s">
+      <c r="E71" s="6" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="72" spans="5:5">
-      <c r="E72" s="3" t="s">
+      <c r="E72" s="6" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="75" spans="19:19">
-      <c r="S75" s="2"/>
+      <c r="S75" s="1"/>
     </row>
     <row r="76" spans="3:5">
       <c r="C76" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D76" s="3" t="s">
+      <c r="D76" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="E76" s="6" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="77" spans="3:3">
-      <c r="C77" s="2"/>
+      <c r="C77" s="1"/>
     </row>
     <row r="78" spans="3:5">
       <c r="C78" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D78" s="3" t="s">
+      <c r="D78" s="6" t="s">
         <v>62</v>
       </c>
       <c r="E78" t="s">
@@ -2360,7 +2737,241 @@
         <v>161</v>
       </c>
     </row>
+    <row r="176" spans="3:6">
+      <c r="C176" s="2"/>
+      <c r="E176" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F176" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="177" spans="5:6">
+      <c r="E177" s="3"/>
+      <c r="F177" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="178" spans="5:6">
+      <c r="E178" s="3"/>
+      <c r="F178" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="179" spans="5:6">
+      <c r="E179" s="3"/>
+      <c r="F179" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="180" spans="5:5">
+      <c r="E180" s="3"/>
+    </row>
+    <row r="181" spans="5:6">
+      <c r="E181" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F181" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="182" spans="6:6">
+      <c r="F182" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="183" spans="6:6">
+      <c r="F183" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="184" spans="6:6">
+      <c r="F184" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="185" spans="6:6">
+      <c r="F185" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="186" spans="6:6">
+      <c r="F186" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="187" spans="6:6">
+      <c r="F187" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="189" spans="5:6">
+      <c r="E189" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F189" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="190" spans="6:6">
+      <c r="F190" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="191" spans="6:6">
+      <c r="F191" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="192" spans="7:7">
+      <c r="G192" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="193" spans="7:7">
+      <c r="G193" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="194" spans="6:6">
+      <c r="F194" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="195" spans="7:7">
+      <c r="G195" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="196" spans="6:6">
+      <c r="F196" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="198" spans="5:6">
+      <c r="E198" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F198" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="199" spans="6:6">
+      <c r="F199" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="200" spans="7:7">
+      <c r="G200" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="201" spans="6:6">
+      <c r="F201" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="202" spans="7:7">
+      <c r="G202" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="203" spans="2:6">
+      <c r="B203" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C203" s="5"/>
+      <c r="F203" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="204" spans="2:7">
+      <c r="B204" s="5"/>
+      <c r="C204" s="5"/>
+      <c r="G204" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="205" spans="6:6">
+      <c r="F205" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="206" spans="7:7">
+      <c r="G206" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="207" spans="6:6">
+      <c r="F207" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="208" spans="7:7">
+      <c r="G208" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="209" spans="6:6">
+      <c r="F209" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="210" spans="7:7">
+      <c r="G210" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="211" spans="6:6">
+      <c r="F211" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="212" spans="7:7">
+      <c r="G212" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="214" spans="5:6">
+      <c r="E214" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F214" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="215" spans="6:6">
+      <c r="F215" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="217" spans="6:6">
+      <c r="F217" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="219" spans="6:10">
+      <c r="F219" t="s">
+        <v>205</v>
+      </c>
+      <c r="J219" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="220" spans="6:6">
+      <c r="F220" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="221" spans="6:6">
+      <c r="F221" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B203:C204"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <drawing r:id="rId1"/>

</xml_diff>